<commit_message>
Adding figures and updated column headers
</commit_message>
<xml_diff>
--- a/excels/IFNgamma.xlsx
+++ b/excels/IFNgamma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alaimos/Desktop/correlation/VVComparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FD55F6-1AFB-EC40-A11B-EFB336BEFF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780E26DB-6F6A-A743-8F3B-F9C9EAADE5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{71883606-44A0-DD4B-AAC5-32B2D3FE2B6E}"/>
   </bookViews>
@@ -38,12 +38,6 @@
     <t>PIK3CB</t>
   </si>
   <si>
-    <t>SARS-CoV2 MOI 2.0</t>
-  </si>
-  <si>
-    <t>Rhinovirus</t>
-  </si>
-  <si>
     <t>IAV</t>
   </si>
   <si>
@@ -84,6 +78,12 @@
   </si>
   <si>
     <t>MYD88</t>
+  </si>
+  <si>
+    <t>SARS-CoV2</t>
+  </si>
+  <si>
+    <t>HRV</t>
   </si>
 </sst>
 </file>
@@ -139,9 +139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +179,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -285,7 +285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,7 +427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,7 +438,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,22 +450,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>4.8202813170000001</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4.4107758820000003</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>4.8202813170000001</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>4.3297205290000003</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>4.4107758820000003</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>4.8202813170000001</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>4.2545988829999999</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>4.4107758820000003</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1.6582280650000001</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4.0573956594611902</v>

</xml_diff>